<commit_message>
modulate factor of hough circle
.
</commit_message>
<xml_diff>
--- a/Open/Kong_Open_True.xlsx
+++ b/Open/Kong_Open_True.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeonSeungYoon\Documents\GitHub\PNU_CalcBean\Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795E19B6-B075-4885-AC24-7515AEC974D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80337494-7C46-421F-84D0-8A5B4BF9A1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
+    <workbookView xWindow="3060" yWindow="2625" windowWidth="12345" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -545,7 +545,7 @@
         <v>44</v>
       </c>
       <c r="C3">
-        <v>225</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -556,7 +556,7 @@
         <v>60</v>
       </c>
       <c r="C4">
-        <v>147</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -567,7 +567,7 @@
         <v>49</v>
       </c>
       <c r="C5">
-        <v>226</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -578,7 +578,7 @@
         <v>129</v>
       </c>
       <c r="C6">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -589,7 +589,7 @@
         <v>39</v>
       </c>
       <c r="C7">
-        <v>151</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -600,7 +600,7 @@
         <v>22</v>
       </c>
       <c r="C8">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -611,7 +611,7 @@
         <v>513</v>
       </c>
       <c r="C9">
-        <v>231</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -622,7 +622,7 @@
         <v>196</v>
       </c>
       <c r="C10">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -633,7 +633,7 @@
         <v>263</v>
       </c>
       <c r="C11">
-        <v>205</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -644,7 +644,7 @@
         <v>170</v>
       </c>
       <c r="C12">
-        <v>200</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>98</v>
       </c>
       <c r="C13">
-        <v>77</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -666,7 +666,7 @@
         <v>379</v>
       </c>
       <c r="C14">
-        <v>222</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -677,7 +677,7 @@
         <v>1600</v>
       </c>
       <c r="C15">
-        <v>221</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -688,7 +688,7 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -699,7 +699,7 @@
         <v>31</v>
       </c>
       <c r="C17">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -710,7 +710,7 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>56</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -721,7 +721,7 @@
         <v>1190</v>
       </c>
       <c r="C19">
-        <v>227</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -732,7 +732,7 @@
         <v>151</v>
       </c>
       <c r="C20">
-        <v>234</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -743,7 +743,7 @@
         <v>108</v>
       </c>
       <c r="C21">
-        <v>231</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>122</v>
       </c>
       <c r="C22">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,7 +765,7 @@
         <v>75</v>
       </c>
       <c r="C23">
-        <v>212</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -776,7 +776,7 @@
         <v>84</v>
       </c>
       <c r="C24">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -787,7 +787,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -798,7 +798,7 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -809,7 +809,7 @@
         <v>1375</v>
       </c>
       <c r="C27">
-        <v>225</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -820,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="C28">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -831,7 +831,7 @@
         <v>1032</v>
       </c>
       <c r="C29">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -842,7 +842,7 @@
         <v>1429</v>
       </c>
       <c r="C30">
-        <v>226</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
         <v>1323</v>
       </c>
       <c r="C31">
-        <v>231</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -864,7 +864,7 @@
         <v>691</v>
       </c>
       <c r="C32">
-        <v>234</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement write result file
.
</commit_message>
<xml_diff>
--- a/Open/Kong_Open_True.xlsx
+++ b/Open/Kong_Open_True.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeonSeungYoon\Documents\GitHub\PNU_CalcBean\Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80337494-7C46-421F-84D0-8A5B4BF9A1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344AF70C-44B6-4907-96EC-9BBC5496DC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="2625" windowWidth="12345" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
+    <workbookView xWindow="6300" yWindow="3420" windowWidth="12345" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>open data index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,58 @@
   </si>
   <si>
     <t>calc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>blur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t17</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>145 이상 측정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -510,15 +562,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81D251E-4845-4DC9-9FC4-82CA64669278}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="14" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +581,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -536,8 +591,14 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -547,8 +608,11 @@
       <c r="C3">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -558,8 +622,14 @@
       <c r="C4">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -569,8 +639,14 @@
       <c r="C5">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -580,8 +656,14 @@
       <c r="C6">
         <v>106</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -591,8 +673,14 @@
       <c r="C7">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -602,8 +690,14 @@
       <c r="C8">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -613,8 +707,14 @@
       <c r="C9">
         <v>198</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>199</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -624,8 +724,14 @@
       <c r="C10">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>176</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -635,8 +741,14 @@
       <c r="C11">
         <v>187</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>181</v>
+      </c>
+      <c r="G11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -646,8 +758,14 @@
       <c r="C12">
         <v>136</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>138</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -657,8 +775,14 @@
       <c r="C13">
         <v>92</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>93</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -668,8 +792,14 @@
       <c r="C14">
         <v>206</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>208</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -679,8 +809,11 @@
       <c r="C15">
         <v>152</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -690,8 +823,11 @@
       <c r="C16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -701,8 +837,11 @@
       <c r="C17">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -712,8 +851,11 @@
       <c r="C18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -723,8 +865,11 @@
       <c r="C19">
         <v>170</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -734,8 +879,11 @@
       <c r="C20">
         <v>88</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -745,8 +893,11 @@
       <c r="C21">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -756,8 +907,11 @@
       <c r="C22">
         <v>101</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -767,8 +921,11 @@
       <c r="C23">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -778,8 +935,11 @@
       <c r="C24">
         <v>78</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -789,8 +949,11 @@
       <c r="C25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -800,8 +963,11 @@
       <c r="C26">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -811,8 +977,11 @@
       <c r="C27">
         <v>195</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -822,8 +991,11 @@
       <c r="C28">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -833,8 +1005,11 @@
       <c r="C29">
         <v>213</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -844,8 +1019,11 @@
       <c r="C30">
         <v>186</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -855,8 +1033,11 @@
       <c r="C31">
         <v>181</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -865,6 +1046,9 @@
       </c>
       <c r="C32">
         <v>186</v>
+      </c>
+      <c r="D32">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implement ensemble algo over 145 beans
.
</commit_message>
<xml_diff>
--- a/Open/Kong_Open_True.xlsx
+++ b/Open/Kong_Open_True.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeonSeungYoon\Documents\GitHub\PNU_CalcBean\Open\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344AF70C-44B6-4907-96EC-9BBC5496DC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6CB609-6238-4F39-AC5A-3B33A5B88AAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6300" yWindow="3420" windowWidth="12345" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
+    <workbookView xWindow="7905" yWindow="1020" windowWidth="12345" windowHeight="11385" xr2:uid="{BB09E280-9D9B-4516-9CDF-9E804A1ADA86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>open data index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -143,10 +143,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>blur</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>t07</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -167,10 +163,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>t25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>t27</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -192,6 +184,41 @@
   </si>
   <si>
     <t>145 이상 측정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t02 : t30 691</t>
+  </si>
+  <si>
+    <t>t03 : t25 1375</t>
+  </si>
+  <si>
+    <t>t04 : t09 263</t>
+  </si>
+  <si>
+    <t>t05 : t27 1032</t>
+  </si>
+  <si>
+    <t>t01 : 기억 안남 ㅋㅋㅋ</t>
+  </si>
+  <si>
+    <t>h01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>h05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -238,11 +265,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -562,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81D251E-4845-4DC9-9FC4-82CA64669278}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -573,15 +603,15 @@
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -591,14 +621,11 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -608,11 +635,14 @@
       <c r="C3">
         <v>43</v>
       </c>
-      <c r="D3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -622,14 +652,20 @@
       <c r="C4">
         <v>59</v>
       </c>
-      <c r="D4">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>59</v>
+      </c>
+      <c r="F4">
+        <v>59</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -639,14 +675,20 @@
       <c r="C5">
         <v>41</v>
       </c>
-      <c r="D5">
-        <v>39</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>41</v>
+      </c>
+      <c r="F5">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -656,14 +698,20 @@
       <c r="C6">
         <v>106</v>
       </c>
-      <c r="D6">
-        <v>104</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>106</v>
+      </c>
+      <c r="F6">
+        <v>106</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -673,14 +721,20 @@
       <c r="C7">
         <v>39</v>
       </c>
-      <c r="D7">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>39</v>
+      </c>
+      <c r="F7">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -690,14 +744,20 @@
       <c r="C8">
         <v>23</v>
       </c>
-      <c r="D8">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>23</v>
+      </c>
+      <c r="F8">
+        <v>23</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -707,14 +767,20 @@
       <c r="C9">
         <v>198</v>
       </c>
-      <c r="D9">
-        <v>199</v>
-      </c>
-      <c r="G9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>1600</v>
+      </c>
+      <c r="F9">
+        <v>1179</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -724,14 +790,20 @@
       <c r="C10">
         <v>176</v>
       </c>
-      <c r="D10">
-        <v>176</v>
-      </c>
-      <c r="G10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>1323</v>
+      </c>
+      <c r="F10">
+        <v>1179</v>
+      </c>
+      <c r="H10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -741,14 +813,20 @@
       <c r="C11">
         <v>187</v>
       </c>
-      <c r="D11">
-        <v>181</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>263</v>
+      </c>
+      <c r="F11">
+        <v>914</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -758,14 +836,20 @@
       <c r="C12">
         <v>136</v>
       </c>
-      <c r="D12">
-        <v>138</v>
-      </c>
-      <c r="G12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>136</v>
+      </c>
+      <c r="F12">
+        <v>136</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -775,14 +859,20 @@
       <c r="C13">
         <v>92</v>
       </c>
-      <c r="D13">
-        <v>93</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>92</v>
+      </c>
+      <c r="F13">
+        <v>92</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -792,14 +882,14 @@
       <c r="C14">
         <v>206</v>
       </c>
-      <c r="D14">
-        <v>208</v>
-      </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>379</v>
+      </c>
+      <c r="F14">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -809,11 +899,14 @@
       <c r="C15">
         <v>152</v>
       </c>
-      <c r="D15">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>196</v>
+      </c>
+      <c r="F15">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -823,11 +916,17 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="H16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -837,11 +936,17 @@
       <c r="C17">
         <v>32</v>
       </c>
-      <c r="D17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <v>32</v>
+      </c>
+      <c r="H17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -851,11 +956,17 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -865,11 +976,17 @@
       <c r="C19">
         <v>170</v>
       </c>
-      <c r="D19">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>263</v>
+      </c>
+      <c r="F19">
+        <v>772</v>
+      </c>
+      <c r="H19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -879,11 +996,17 @@
       <c r="C20">
         <v>88</v>
       </c>
-      <c r="D20">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>85</v>
+      </c>
+      <c r="F20">
+        <v>85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -893,11 +1016,14 @@
       <c r="C21">
         <v>91</v>
       </c>
-      <c r="D21">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>91</v>
+      </c>
+      <c r="F21">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -907,11 +1033,14 @@
       <c r="C22">
         <v>101</v>
       </c>
-      <c r="D22">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>101</v>
+      </c>
+      <c r="F22">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -921,11 +1050,14 @@
       <c r="C23">
         <v>72</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -935,11 +1067,14 @@
       <c r="C24">
         <v>78</v>
       </c>
-      <c r="D24">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>79</v>
+      </c>
+      <c r="F24">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -949,11 +1084,14 @@
       <c r="C25">
         <v>11</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>11</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -963,11 +1101,14 @@
       <c r="C26">
         <v>24</v>
       </c>
-      <c r="D26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>24</v>
+      </c>
+      <c r="F26">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -977,11 +1118,14 @@
       <c r="C27">
         <v>195</v>
       </c>
-      <c r="D27">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>263</v>
+      </c>
+      <c r="F27">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -991,11 +1135,14 @@
       <c r="C28">
         <v>8</v>
       </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1005,11 +1152,14 @@
       <c r="C29">
         <v>213</v>
       </c>
-      <c r="D29">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E29">
+        <v>379</v>
+      </c>
+      <c r="F29">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1019,11 +1169,14 @@
       <c r="C30">
         <v>186</v>
       </c>
-      <c r="D30">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>263</v>
+      </c>
+      <c r="F30">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1033,11 +1186,14 @@
       <c r="C31">
         <v>181</v>
       </c>
-      <c r="D31">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>379</v>
+      </c>
+      <c r="F31">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1047,8 +1203,79 @@
       <c r="C32">
         <v>186</v>
       </c>
-      <c r="D32">
-        <v>190</v>
+      <c r="E32">
+        <v>379</v>
+      </c>
+      <c r="F32">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33">
+        <v>263</v>
+      </c>
+      <c r="F33">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34">
+        <v>691</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="E34">
+        <v>1032</v>
+      </c>
+      <c r="F34">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35">
+        <v>1375</v>
+      </c>
+      <c r="E35">
+        <v>263</v>
+      </c>
+      <c r="F35">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36">
+        <v>263</v>
+      </c>
+      <c r="E36">
+        <v>1323</v>
+      </c>
+      <c r="F36">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37">
+        <v>1032</v>
+      </c>
+      <c r="E37">
+        <v>1032</v>
+      </c>
+      <c r="F37">
+        <v>1011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>